<commit_message>
snapshot: point de référence avant nouvelles modifications
</commit_message>
<xml_diff>
--- a/data/bic_codes.xlsx
+++ b/data/bic_codes.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Stage pro BEAC\Work\Projet Suivi des RC\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\alannmatis\pdf-extractor\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15320" windowHeight="4970"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="325">
   <si>
     <t>Nom abrégé de participant</t>
   </si>
@@ -978,6 +978,27 @@
   </si>
   <si>
     <t>16.08.2021 10:25:23</t>
+  </si>
+  <si>
+    <t>Pays</t>
+  </si>
+  <si>
+    <t>Cameroun</t>
+  </si>
+  <si>
+    <t>Congo</t>
+  </si>
+  <si>
+    <t>Gabon</t>
+  </si>
+  <si>
+    <t>Guinée Equatoriale</t>
+  </si>
+  <si>
+    <t>RCA</t>
+  </si>
+  <si>
+    <t>Tchad</t>
   </si>
 </sst>
 </file>
@@ -1335,10 +1356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I76"/>
+  <dimension ref="A1:J76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1346,15 +1367,16 @@
     <col min="1" max="1" width="24.7265625" customWidth="1"/>
     <col min="2" max="2" width="23.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.26953125" customWidth="1"/>
-    <col min="4" max="4" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6328125" customWidth="1"/>
+    <col min="5" max="5" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
@@ -1365,25 +1387,28 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1393,26 +1418,29 @@
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E2" s="3">
         <v>8128</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>63</v>
       </c>
@@ -1422,26 +1450,29 @@
       <c r="C3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E3" s="3">
         <v>8101</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -1451,26 +1482,29 @@
       <c r="C4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E4" s="3">
         <v>8102</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
@@ -1480,26 +1514,29 @@
       <c r="C5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E5" s="3">
         <v>8127</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>57</v>
       </c>
@@ -1509,24 +1546,27 @@
       <c r="C6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E6" s="3">
         <v>9910</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="H6" s="3"/>
       <c r="I6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
@@ -1536,26 +1576,29 @@
       <c r="C7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E7" s="3">
         <v>8123</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>37</v>
       </c>
@@ -1565,26 +1608,29 @@
       <c r="C8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E8" s="3">
         <v>8122</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>58</v>
       </c>
@@ -1594,26 +1640,29 @@
       <c r="C9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E9" s="3">
         <v>8125</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="39" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="39" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>59</v>
       </c>
@@ -1623,26 +1672,29 @@
       <c r="C10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E10" s="3">
         <v>8104</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>60</v>
       </c>
@@ -1652,26 +1704,29 @@
       <c r="C11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E11" s="3">
         <v>1410</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>50</v>
       </c>
@@ -1681,26 +1736,29 @@
       <c r="C12" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E12" s="3">
         <v>8109</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>61</v>
       </c>
@@ -1710,26 +1768,29 @@
       <c r="C13" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E13" s="3">
         <v>8110</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="J13" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>64</v>
       </c>
@@ -1739,26 +1800,29 @@
       <c r="C14" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E14" s="3">
         <v>8108</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>104</v>
       </c>
@@ -1768,26 +1832,29 @@
       <c r="C15" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E15" s="3">
         <v>8126</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>71</v>
       </c>
@@ -1797,26 +1864,29 @@
       <c r="C16" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E16" s="3">
         <v>1001</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F16" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="I16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>76</v>
       </c>
@@ -1826,26 +1896,29 @@
       <c r="C17" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E17" s="3">
         <v>8112</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="J17" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>80</v>
       </c>
@@ -1855,26 +1928,29 @@
       <c r="C18" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E18" s="3">
         <v>8119</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>84</v>
       </c>
@@ -1884,26 +1960,29 @@
       <c r="C19" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E19" s="3">
         <v>8111</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>88</v>
       </c>
@@ -1913,26 +1992,29 @@
       <c r="C20" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E20" s="3">
         <v>8115</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>92</v>
       </c>
@@ -1942,26 +2024,29 @@
       <c r="C21" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E21" s="3">
         <v>8118</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="J21" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>96</v>
       </c>
@@ -1971,26 +2056,29 @@
       <c r="C22" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E22" s="3">
         <v>8103</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>100</v>
       </c>
@@ -2000,26 +2088,29 @@
       <c r="C23" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E23" s="3">
         <v>8120</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F23" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="J23" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>105</v>
       </c>
@@ -2029,26 +2120,29 @@
       <c r="C24" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E24" s="3">
         <v>8409</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>109</v>
       </c>
@@ -2058,26 +2152,29 @@
       <c r="C25" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E25" s="3">
         <v>8413</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>113</v>
       </c>
@@ -2087,24 +2184,27 @@
       <c r="C26" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E26" s="3">
         <v>9940</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="H26" s="3"/>
       <c r="I26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>116</v>
       </c>
@@ -2114,26 +2214,29 @@
       <c r="C27" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E27" s="3">
         <v>8401</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>120</v>
       </c>
@@ -2143,26 +2246,29 @@
       <c r="C28" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E28" s="3">
         <v>8407</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F28" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>124</v>
       </c>
@@ -2172,26 +2278,29 @@
       <c r="C29" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E29" s="3">
         <v>8410</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>14</v>
+      <c r="G29" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>129</v>
       </c>
@@ -2201,26 +2310,29 @@
       <c r="C30" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E30" s="3">
         <v>8414</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>133</v>
       </c>
@@ -2230,26 +2342,29 @@
       <c r="C31" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E31" s="3">
         <v>9114</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F31" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H31" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="I31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>138</v>
       </c>
@@ -2259,26 +2374,29 @@
       <c r="C32" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E32" s="3">
         <v>8404</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F32" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I32" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="3" t="s">
+      <c r="J32" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>142</v>
       </c>
@@ -2288,26 +2406,29 @@
       <c r="C33" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E33" s="3">
         <v>8408</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F33" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I33" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="J33" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>146</v>
       </c>
@@ -2317,26 +2438,29 @@
       <c r="C34" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E34" s="3">
         <v>8405</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F34" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J34" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>152</v>
       </c>
@@ -2346,26 +2470,29 @@
       <c r="C35" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E35" s="3">
         <v>8406</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F35" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G35" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H35" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="I35" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>156</v>
       </c>
@@ -2375,26 +2502,29 @@
       <c r="C36" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E36" s="3">
         <v>4406</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F36" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I36" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>160</v>
       </c>
@@ -2404,26 +2534,29 @@
       <c r="C37" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E37" s="3">
         <v>8412</v>
       </c>
-      <c r="E37" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F37" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>164</v>
       </c>
@@ -2433,26 +2566,29 @@
       <c r="C38" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E38" s="3">
         <v>4001</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F38" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G38" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H38" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="I38" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J38" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>168</v>
       </c>
@@ -2462,26 +2598,29 @@
       <c r="C39" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E39" s="3">
         <v>8411</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F39" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I39" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J39" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>172</v>
       </c>
@@ -2491,26 +2630,29 @@
       <c r="C40" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E40" s="3">
         <v>8514</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="F40" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="G40" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="G40" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="H40" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I40" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="I40" s="3" t="s">
+      <c r="J40" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>177</v>
       </c>
@@ -2520,26 +2662,29 @@
       <c r="C41" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E41" s="3">
         <v>8503</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="F41" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F41" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>14</v>
+      <c r="G41" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I41" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J41" s="3" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>181</v>
       </c>
@@ -2549,24 +2694,27 @@
       <c r="C42" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E42" s="3">
         <v>9950</v>
       </c>
-      <c r="E42" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F42" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="H42" s="3"/>
       <c r="I42" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J42" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>184</v>
       </c>
@@ -2576,26 +2724,29 @@
       <c r="C43" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E43" s="3">
         <v>8504</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F43" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H43" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I43" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I43" s="3" t="s">
+      <c r="J43" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="39" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="39" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>188</v>
       </c>
@@ -2605,26 +2756,29 @@
       <c r="C44" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E44" s="3">
         <v>8506</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F44" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H44" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I44" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I44" s="3" t="s">
+      <c r="J44" s="3" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>192</v>
       </c>
@@ -2634,26 +2788,29 @@
       <c r="C45" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E45" s="3">
         <v>8519</v>
       </c>
-      <c r="E45" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F45" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H45" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I45" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I45" s="3" t="s">
+      <c r="J45" s="3" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>196</v>
       </c>
@@ -2663,26 +2820,29 @@
       <c r="C46" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E46" s="3">
         <v>8509</v>
       </c>
-      <c r="E46" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F46" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H46" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I46" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I46" s="3" t="s">
+      <c r="J46" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>200</v>
       </c>
@@ -2692,26 +2852,29 @@
       <c r="C47" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E47" s="3">
         <v>8516</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F47" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H47" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I47" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I47" s="3" t="s">
+      <c r="J47" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>204</v>
       </c>
@@ -2721,26 +2884,29 @@
       <c r="C48" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E48" s="3">
         <v>8511</v>
       </c>
-      <c r="E48" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F48" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H48" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I48" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I48" s="3" t="s">
+      <c r="J48" s="3" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>208</v>
       </c>
@@ -2750,26 +2916,29 @@
       <c r="C49" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E49" s="3">
         <v>5001</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F49" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G49" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H49" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H49" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="I49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J49" s="3" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>212</v>
       </c>
@@ -2779,26 +2948,29 @@
       <c r="C50" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E50" s="3">
         <v>8512</v>
       </c>
-      <c r="E50" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F50" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H50" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I50" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I50" s="3" t="s">
+      <c r="J50" s="3" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>216</v>
       </c>
@@ -2808,26 +2980,29 @@
       <c r="C51" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E51" s="3">
         <v>8517</v>
       </c>
-      <c r="E51" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F51" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I51" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J51" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>220</v>
       </c>
@@ -2837,26 +3012,29 @@
       <c r="C52" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E52" s="3">
         <v>8604</v>
       </c>
-      <c r="E52" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F52" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H52" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I52" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J52" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>224</v>
       </c>
@@ -2866,24 +3044,27 @@
       <c r="C53" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D53" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E53" s="3">
         <v>9960</v>
       </c>
-      <c r="E53" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F53" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G53" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="H53" s="3"/>
       <c r="I53" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J53" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>227</v>
       </c>
@@ -2893,26 +3074,29 @@
       <c r="C54" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D54" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E54" s="3">
         <v>8601</v>
       </c>
-      <c r="E54" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F54" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H54" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I54" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J54" s="3" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>231</v>
       </c>
@@ -2922,26 +3106,29 @@
       <c r="C55" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D55" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E55" s="3">
         <v>8602</v>
       </c>
-      <c r="E55" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F55" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H55" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I55" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J55" s="3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>235</v>
       </c>
@@ -2951,26 +3138,29 @@
       <c r="C56" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="D56" s="3">
+      <c r="D56" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E56" s="3">
         <v>8605</v>
       </c>
-      <c r="E56" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F56" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H56" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I56" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I56" s="3" t="s">
+      <c r="J56" s="3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>239</v>
       </c>
@@ -2980,26 +3170,29 @@
       <c r="C57" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="D57" s="3">
+      <c r="D57" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E57" s="3">
         <v>8603</v>
       </c>
-      <c r="E57" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F57" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I57" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J57" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>243</v>
       </c>
@@ -3009,26 +3202,29 @@
       <c r="C58" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="D58" s="3">
+      <c r="D58" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E58" s="3">
         <v>6001</v>
       </c>
-      <c r="E58" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F58" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G58" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H58" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H58" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="I58" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J58" s="3" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>247</v>
       </c>
@@ -3038,24 +3234,27 @@
       <c r="C59" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="D59" s="3">
+      <c r="D59" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E59" s="3">
         <v>9930</v>
       </c>
-      <c r="E59" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F59" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G59" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="H59" s="3"/>
       <c r="I59" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J59" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>250</v>
       </c>
@@ -3065,26 +3264,29 @@
       <c r="C60" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="D60" s="3">
+      <c r="D60" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E60" s="3">
         <v>8304</v>
       </c>
-      <c r="E60" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F60" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H60" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I60" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J60" s="3" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>254</v>
       </c>
@@ -3094,26 +3296,29 @@
       <c r="C61" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="D61" s="3">
+      <c r="D61" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E61" s="3">
         <v>8302</v>
       </c>
-      <c r="E61" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F61" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G61" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H61" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I61" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J61" s="3" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
         <v>258</v>
       </c>
@@ -3123,26 +3328,29 @@
       <c r="C62" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="D62" s="3">
+      <c r="D62" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E62" s="3">
         <v>8303</v>
       </c>
-      <c r="E62" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F62" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H62" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I62" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J62" s="3" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>262</v>
       </c>
@@ -3152,26 +3360,29 @@
       <c r="C63" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="D63" s="3">
+      <c r="D63" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E63" s="3">
         <v>8301</v>
       </c>
-      <c r="E63" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F63" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H63" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I63" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I63" s="3" t="s">
+      <c r="J63" s="3" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>266</v>
       </c>
@@ -3181,26 +3392,29 @@
       <c r="C64" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="D64" s="3">
+      <c r="D64" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E64" s="3">
         <v>3001</v>
       </c>
-      <c r="E64" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F64" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G64" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H64" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H64" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="I64" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J64" s="3" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>270</v>
       </c>
@@ -3210,26 +3424,29 @@
       <c r="C65" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="D65" s="3">
+      <c r="D65" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E65" s="3">
         <v>8216</v>
       </c>
-      <c r="E65" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F65" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H65" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I65" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J65" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>274</v>
       </c>
@@ -3239,24 +3456,27 @@
       <c r="C66" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="D66" s="3">
+      <c r="D66" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E66" s="3">
         <v>9920</v>
       </c>
-      <c r="E66" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F66" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G66" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="H66" s="3"/>
       <c r="I66" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J66" s="3" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>278</v>
       </c>
@@ -3266,26 +3486,29 @@
       <c r="C67" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="D67" s="3">
+      <c r="D67" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E67" s="3">
         <v>8201</v>
       </c>
-      <c r="E67" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F67" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G67" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H67" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I67" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J67" s="3" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
         <v>282</v>
       </c>
@@ -3295,26 +3518,29 @@
       <c r="C68" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="D68" s="3">
+      <c r="D68" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E68" s="3">
         <v>8202</v>
       </c>
-      <c r="E68" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F68" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G68" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H68" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I68" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I68" s="3" t="s">
+      <c r="J68" s="3" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>286</v>
       </c>
@@ -3324,26 +3550,29 @@
       <c r="C69" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="D69" s="3">
+      <c r="D69" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E69" s="3">
         <v>8215</v>
       </c>
-      <c r="E69" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F69" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G69" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H69" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I69" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J69" s="3" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>290</v>
       </c>
@@ -3353,26 +3582,29 @@
       <c r="C70" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="D70" s="3">
+      <c r="D70" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E70" s="3">
         <v>8205</v>
       </c>
-      <c r="E70" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F70" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G70" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H70" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I70" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J70" s="3" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
         <v>294</v>
       </c>
@@ -3382,26 +3614,29 @@
       <c r="C71" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="D71" s="3">
+      <c r="D71" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E71" s="3">
         <v>8206</v>
       </c>
-      <c r="E71" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F71" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G71" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H71" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I71" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J71" s="3" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>298</v>
       </c>
@@ -3411,26 +3646,29 @@
       <c r="C72" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="D72" s="3">
+      <c r="D72" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E72" s="3">
         <v>8203</v>
       </c>
-      <c r="E72" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F72" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H72" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I72" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I72" s="3" t="s">
+      <c r="J72" s="3" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
         <v>302</v>
       </c>
@@ -3440,26 +3678,29 @@
       <c r="C73" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="D73" s="3">
+      <c r="D73" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E73" s="3">
         <v>8207</v>
       </c>
-      <c r="E73" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F73" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G73" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H73" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I73" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J73" s="3" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
         <v>306</v>
       </c>
@@ -3469,26 +3710,29 @@
       <c r="C74" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="D74" s="3">
+      <c r="D74" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E74" s="3">
         <v>8208</v>
       </c>
-      <c r="E74" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F74" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G74" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H74" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I74" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J74" s="3" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>310</v>
       </c>
@@ -3498,26 +3742,29 @@
       <c r="C75" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="D75" s="3">
+      <c r="D75" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E75" s="3">
         <v>2001</v>
       </c>
-      <c r="E75" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F75" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G75" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H75" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H75" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="I75" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J75" s="3" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
         <v>314</v>
       </c>
@@ -3527,22 +3774,25 @@
       <c r="C76" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="D76" s="3">
+      <c r="D76" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E76" s="3">
         <v>8213</v>
       </c>
-      <c r="E76" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F76" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G76" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H76" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I76" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J76" s="3" t="s">
         <v>317</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: refactored donneur_dordre display & added country lookup
- Split donneur_dordre into code_donneur_dordre (code only) and donneur_dordre (name only)
- Added map_code_to_country() function in bic_utils to lookup country by BIC code
- Added _fill_country_from_code() in mt_multi to auto-fill pays_iso3 from code when empty
- Updated create_workbook() to show both columns in Excel export
- Updated streamlit display to show new 'Code du donneur d'ordre' column
- Both Streamlit and Excel outputs now display identically
</commit_message>
<xml_diff>
--- a/data/bic_codes.xlsx
+++ b/data/bic_codes.xlsx
@@ -983,22 +983,22 @@
     <t>Pays</t>
   </si>
   <si>
-    <t>Cameroun</t>
-  </si>
-  <si>
-    <t>Congo</t>
-  </si>
-  <si>
-    <t>Gabon</t>
-  </si>
-  <si>
-    <t>Guinée Equatoriale</t>
-  </si>
-  <si>
-    <t>RCA</t>
-  </si>
-  <si>
-    <t>Tchad</t>
+    <t>CMR</t>
+  </si>
+  <si>
+    <t>CNG</t>
+  </si>
+  <si>
+    <t>GAB</t>
+  </si>
+  <si>
+    <t>GNQ</t>
+  </si>
+  <si>
+    <t>CAF</t>
+  </si>
+  <si>
+    <t>TCD</t>
   </si>
 </sst>
 </file>
@@ -1358,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3064,7 +3064,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="26" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>227</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="26" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>231</v>
       </c>

</xml_diff>

<commit_message>
feat: Stocker et afficher BEACCMCX091 séparément + Mise à jour codes BIC
- Les messages BEACCMCX091 ne sont plus rejetés mais stockés dans une liste séparée
- Ajout d'une feuille Excel 'BEACCMCX091' après le summary
- Modification de mt_multi.py pour retourner 3 valeurs (rows, beaccmcx091_rows, missing_codes)
- Mise à jour de extract_dispatch() et create_workbook()
- Interface utilisateur mise à jour pour afficher les BEACCMCX091
- Mise à jour du fichier bic_codes.xlsx avec de nouvelles entités
</commit_message>
<xml_diff>
--- a/data/bic_codes.xlsx
+++ b/data/bic_codes.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="15320" windowHeight="4970"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="167">
   <si>
     <t>Code BIC</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Noms</t>
   </si>
   <si>
-    <t>Afriland First Bank Cameroun</t>
-  </si>
-  <si>
     <t>Commercial Bank of Cameroun</t>
   </si>
   <si>
@@ -161,9 +158,6 @@
     <t>UNAFCMCX</t>
   </si>
   <si>
-    <t>Credit Communautaire d’Afrique/ Cameroun</t>
-  </si>
-  <si>
     <t>BANQUE CONGOLAISE DE L’HABITAT</t>
   </si>
   <si>
@@ -242,12 +236,6 @@
     <t>SPECCGCG</t>
   </si>
   <si>
-    <t>Société Générale Congo</t>
-  </si>
-  <si>
-    <t>SOGECGCG</t>
-  </si>
-  <si>
     <t>TRESOR DU CONGO</t>
   </si>
   <si>
@@ -284,12 +272,6 @@
     <t>BGFIGALI</t>
   </si>
   <si>
-    <t>Banque Internationale pour le Commerce et l'Industrie du GABON</t>
-  </si>
-  <si>
-    <t>BICIGALX</t>
-  </si>
-  <si>
     <t>Banque Postale du Gabon</t>
   </si>
   <si>
@@ -392,9 +374,6 @@
     <t>BPMCCFCF</t>
   </si>
   <si>
-    <t>Commercial Bank Centrafrique</t>
-  </si>
-  <si>
     <t>CBCACFCF</t>
   </si>
   <si>
@@ -464,12 +443,6 @@
     <t>ORBKTDND</t>
   </si>
   <si>
-    <t>Société Générale Tchad</t>
-  </si>
-  <si>
-    <t>SOGETDND</t>
-  </si>
-  <si>
     <t>TRESOR DU TCHAD</t>
   </si>
   <si>
@@ -501,6 +474,57 @@
   </si>
   <si>
     <t>TCD</t>
+  </si>
+  <si>
+    <t>AGBDCMCX</t>
+  </si>
+  <si>
+    <t>Afriland First Bank</t>
+  </si>
+  <si>
+    <t>LA REGIONALE BANK</t>
+  </si>
+  <si>
+    <t>LREGCMCX</t>
+  </si>
+  <si>
+    <t>Africa Golden Bank SA</t>
+  </si>
+  <si>
+    <t>Credit Communautaire d'Afrique</t>
+  </si>
+  <si>
+    <t>AFG BANK GABON</t>
+  </si>
+  <si>
+    <t>AFGGGALX</t>
+  </si>
+  <si>
+    <t>Banque pour le Commerce et l’Entreprenariat du Gabon</t>
+  </si>
+  <si>
+    <t>BCGBGALI</t>
+  </si>
+  <si>
+    <t>CAISSE DES DEPOTS ET CONSIGNATIONS</t>
+  </si>
+  <si>
+    <t>CDCGGALI</t>
+  </si>
+  <si>
+    <t>BGFI Centrafrique</t>
+  </si>
+  <si>
+    <t>African Development and Investment Congo</t>
+  </si>
+  <si>
+    <t>BRAZCGCG</t>
+  </si>
+  <si>
+    <t>CORIS BANK INTERNATIONAL TCHAD</t>
+  </si>
+  <si>
+    <t>CORITDND</t>
   </si>
 </sst>
 </file>
@@ -564,7 +588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -577,6 +601,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -858,20 +885,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.7265625" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" customWidth="1"/>
-    <col min="3" max="3" width="7.08984375" customWidth="1"/>
+    <col min="1" max="1" width="54.36328125" customWidth="1"/>
+    <col min="2" max="3" width="29.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -879,7 +903,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -890,825 +914,868 @@
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>25</v>
+        <v>154</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>151</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="26" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="39" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="C10" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="26" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="C11" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="26" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C15" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="26" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="26" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="C16" s="3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="26" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="C18" s="3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>36</v>
+        <v>153</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C24" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="26" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="26" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="26" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="C25" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>54</v>
+        <v>100</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>55</v>
+        <v>101</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
-        <v>56</v>
+      <c r="A29" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>58</v>
+        <v>104</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>61</v>
+        <v>107</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>62</v>
+        <v>108</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>64</v>
+        <v>156</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>65</v>
+        <v>157</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>76</v>
+        <v>158</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>77</v>
+        <v>159</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>78</v>
+        <v>160</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="39" x14ac:dyDescent="0.35">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
-        <v>94</v>
+        <v>162</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
-        <v>104</v>
+        <v>163</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>105</v>
+        <v>164</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>107</v>
+        <v>45</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" s="4" t="s">
-        <v>108</v>
+      <c r="A55" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>109</v>
+        <v>47</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
-        <v>110</v>
+        <v>48</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>111</v>
+        <v>49</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>113</v>
+        <v>51</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
-        <v>114</v>
+        <v>52</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>115</v>
+        <v>53</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>117</v>
+        <v>55</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
-        <v>118</v>
+        <v>56</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>119</v>
+        <v>57</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
-        <v>120</v>
+        <v>58</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>121</v>
+        <v>59</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
-        <v>122</v>
+        <v>60</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>123</v>
+        <v>61</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
-        <v>124</v>
+        <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
-        <v>126</v>
+        <v>64</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>127</v>
+        <v>65</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
-        <v>128</v>
+        <v>66</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>129</v>
+        <v>67</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
-        <v>130</v>
+        <v>68</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>131</v>
+        <v>69</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
-        <v>132</v>
+        <v>70</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>133</v>
+        <v>71</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
-        <v>134</v>
+        <v>72</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>135</v>
+        <v>73</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>158</v>
+        <v>124</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>158</v>
+        <v>126</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>158</v>
+        <v>128</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>158</v>
+        <v>130</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>158</v>
+        <v>132</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="B75" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C75" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>158</v>
+        <v>134</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>